<commit_message>
add answer for tag บอทโง่
</commit_message>
<xml_diff>
--- a/data/response.xlsx
+++ b/data/response.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -558,9 +558,27 @@
         <v>สบายดีงับบ</v>
       </c>
     </row>
+    <row r="20" xml:space="preserve">
+      <c r="A20" t="str">
+        <v>บอทโง่</v>
+      </c>
+      <c r="B20" t="str" xml:space="preserve">
+        <v xml:space="preserve">ไม่เข้าจายย พิมพ์ตามหัวข้อนี้หน่อยน้า
+        1. กฎหมายที่สำคัญ
+        2. การฝากร้าน
+        3. ขั้นตอนการจดทะเบียนพาณิชย์ค้าขายออนไลน์
+        4. เริ่มต้นเปิดร้าน
+        5. ร้านแบบไหนต้องจดทะเบียนอิเล็กทรอนิกส์
+        6. กม.ขายของออนไลน์กับกม.คุ้มครองผู้บริโภค
+        7. สินค้าที่ห้ามขายออนไลน์
+        8. รายละเอียดที่ต้องแสดงในการขาย
+        9. การเสียภาษี
+        10. การขายตรง</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B19"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B20"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add more tag , question and response
</commit_message>
<xml_diff>
--- a/data/response.xlsx
+++ b/data/response.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -510,14 +510,6 @@
         <v>สวัสดีค้าบบ</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>ทักทาย</v>
-      </c>
-      <c r="B14" t="str">
-        <v>สวัสดีค้าาา</v>
-      </c>
-    </row>
     <row r="15">
       <c r="A15" t="str">
         <v>ทักทาย</v>
@@ -558,27 +550,49 @@
         <v>สบายดีงับบ</v>
       </c>
     </row>
-    <row r="20" xml:space="preserve">
-      <c r="A20" t="str">
+    <row r="21">
+      <c r="A21" t="str">
+        <v>easter</v>
+      </c>
+      <c r="B21" t="str">
+        <v>จารย์โบ๊ท No1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
         <v>บอทโง่</v>
       </c>
-      <c r="B20" t="str" xml:space="preserve">
-        <v xml:space="preserve">ไม่เข้าจายย พิมพ์ตามหัวข้อนี้หน่อยน้า
-        1. กฎหมายที่สำคัญ
-        2. การฝากร้าน
-        3. ขั้นตอนการจดทะเบียนพาณิชย์ค้าขายออนไลน์
-        4. เริ่มต้นเปิดร้าน
-        5. ร้านแบบไหนต้องจดทะเบียนอิเล็กทรอนิกส์
-        6. กม.ขายของออนไลน์กับกม.คุ้มครองผู้บริโภค
-        7. สินค้าที่ห้ามขายออนไลน์
-        8. รายละเอียดที่ต้องแสดงในการขาย
-        9. การเสียภาษี
-        10. การขายตรง</v>
+      <c r="B23" t="str">
+        <v>เราขอโทษ</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>ชมบอท</v>
+      </c>
+      <c r="B25" t="str">
+        <v>ขอบคุณค้าบ</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>ทำอะไร</v>
+      </c>
+      <c r="B27" t="str">
+        <v>รอให้ความช่วยเหลือด้านกฎหมายค้าบ</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>ชื่ออะไร</v>
+      </c>
+      <c r="B29" t="str">
+        <v>น้องบอท</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B20"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B29"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add more question and tag
</commit_message>
<xml_diff>
--- a/data/response.xlsx
+++ b/data/response.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -393,15 +393,14 @@
         <v>หนึ่ง</v>
       </c>
       <c r="B2" t="str" xml:space="preserve">
-        <v xml:space="preserve">กฎหมายทะเบียนพาณิชย์_x000d_
-กฎหมายลิขสิทธิ์ พ.ศ.2537_x000d_
-กฎหมายขายตรงและตลาดขายตรง พ.ศ.2545_x000d_
-กฎหมายธุรกรรมทางอิเล็กทรอนิกส์ พ.ศ.2544_x000d_
-กฎหมายคุ้มครองผู้บริโภค พ.ศ.2522_x000d_
-กฎหมายว่าด้วยเกี่ยวกับการกระทำผิดเกี่ยวกับคอมพิวเตอร์ พ.ศ.2560_x000d_
-กฎหมายภาษี (ประมวลรัษฎากร)_x000d_
-พระราชบัญญัติการแข่งขันทางการค้า_x000d_
-กฎหมายว่าด้วยราคาสินค้าและบริการ พ.ศ.2542_x000d_
+        <v xml:space="preserve">กฎหมายทะเบียนพาณิชย์กฎหมายลิขสิทธิ์ พ.ศ.2537
+กฎหมายขายตรงและตลาดขายตรง พ.ศ.2545
+กฎหมายธุรกรรมทางอิเล็กทรอนิกส์ พ.ศ.2544
+กฎหมายคุ้มครองผู้บริโภค พ.ศ.2522
+กฎหมายว่าด้วยเกี่ยวกับการกระทำผิดเกี่ยวกับคอมพิวเตอร์ พ.ศ.2560
+กฎหมายภาษี (ประมวลรัษฎากร)
+พระราชบัญญัติการแข่งขันทางการค้า
+กฎหมายว่าด้วยราคาสินค้าและบริการ พ.ศ.2542
 กฎหมายผลิตภัณฑ์อาหารและยา </v>
       </c>
     </row>
@@ -550,14 +549,6 @@
         <v>สบายดีงับบ</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="str">
-        <v>easter</v>
-      </c>
-      <c r="B21" t="str">
-        <v>จารย์โบ๊ท No1</v>
-      </c>
-    </row>
     <row r="23">
       <c r="A23" t="str">
         <v>บอทโง่</v>
@@ -587,12 +578,29 @@
         <v>ชื่ออะไร</v>
       </c>
       <c r="B29" t="str">
-        <v>น้องบอท</v>
+        <v>น้องบอทค้าบบ</v>
+      </c>
+    </row>
+    <row r="31" xml:space="preserve">
+      <c r="A31" t="str">
+        <v>หัวข้อ</v>
+      </c>
+      <c r="B31" t="str" xml:space="preserve">
+        <v xml:space="preserve">1. กฎหมายที่สำคัญ
+2. การฝากร้าน
+3. ขั้นตอนการจดทะเบียนพาณิชย์ค้าขายออนไลน์
+4. เริ่มต้นเปิดร้าน
+5. ร้านแบบไหนต้องจดทะเบียนอิเล็กทรอนิกส์
+6. กม.ขายของออนไลน์กับกม.คุ้มครองผู้บริโภค
+7. สินค้าที่ห้ามขายออนไลน์
+8. รายละเอียดที่ต้องแสดงในการขาย
+9. การเสียภาษี
+10. การขายตรงได้ไหม</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B29"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B31"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add more tag and keywords
</commit_message>
<xml_diff>
--- a/data/response.xlsx
+++ b/data/response.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Projects\baisd\chat_bot_team\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F85CA08-B563-465C-9686-2B0D5F8C8F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E75B08-0695-44AE-AF3C-B7DAD6FD19D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>tag</t>
   </si>
@@ -186,6 +186,15 @@
   </si>
   <si>
     <t>ยินดีจ้า</t>
+  </si>
+  <si>
+    <t>มีคำถาม</t>
+  </si>
+  <si>
+    <t>ถามได้เลยค้าบบ</t>
+  </si>
+  <si>
+    <t>ถามมาได้เลยค้าบบ</t>
   </si>
 </sst>
 </file>
@@ -565,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -773,6 +782,22 @@
         <v>43</v>
       </c>
     </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
update responsce by make it shorter response
</commit_message>
<xml_diff>
--- a/data/response.xlsx
+++ b/data/response.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Projects\baisd\chat_bot_team\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB526C86-0C0C-447F-A896-7D1AA32A5E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E0AF35-6B08-4CDB-9247-057C84ACEAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -197,13 +197,13 @@
 9. กฎหมายผลิตภัณฑ์อาหารและยา </t>
   </si>
   <si>
-    <t>การแชร์รูปภาพหรือข้อความต่างๆ เกี่ยวกับร้านค้าออนไลน์ของตนในพื้นที่โซเซียลมีดีของผู้อื่นผิดกฎหมายนะครับ</t>
-  </si>
-  <si>
     <t>ไม่สามารถขายตรงได้ เนื่องจาก 
 1. กรณีเจ้าของเว็บไซต์ที่จดทะเบียนเว็บไซต์ไว้เพื่อขายสินค้าของตนเองก็ดีหรือเป็นคนกลางในการนำ สินค้าของบุคคลอื่นมาขายผ่านหน้าเว็บไซต์ก็ดี มีหน้าที่โดยตรงในการต้องไปจดทะเบียนต่อสำนักงานคณะกรรมการคุ้มครองผู้บริโภค ทั้งนี้เจ้าของเว็บไซต์จะต้องแจ้ง รายละเอียดเกี่ยวกับชนิดหรือประเภทของสินค้า ชื่อที่อยู่ของเจ้าของ ผลิตภัณฑ์ วิธีการซื้อขาย เงื่อนไขต่างๆ ให้ นายทะเบียนการประกอบธุรกิจตลาดแบบตรงทราบด้วย หากมีปัญหาการผิดสัญญาก็ดี สินค้าไม่ได้มาตรฐาน หรือไม่ปลอดภัยก็ดีสำนักงานคณะกรรมการคุ้มครองผู้บริโภคย่อมสามารถตรวจสอบและติดตามผู้ต้องรับผิดได้
 2. กรณีบริษัทห้างร้านหรือบุคคลธรรมดาที่เป็นเจ้าของผลิตภัณฑ์ ไม่ว่าจะเป็นผู้ผลิต ผู้นำเข้าหรือผู้แทนจำหน่าย หรือผู้ขาย หากจดทะเบียนเว็บไซต์เพื่อค้าขายสินค้าผ่านอินเตอร์เน็ตเป็นของตนเอง โดยไม่ผ่านเว็บไซต์ที่เป็นสื่อกลางดังที่กล่าวมาในข้อ 1.1 ดังนั้นบริษัท ห้างร้าน หรือบุคคลธรรมดาที่เป็นเจ้าของ ผลิตภัณฑ์จะต้องเป็นผู้มีหน้าที่ต้องไปจดทะเบียนการประกอบธุรกิจตลาดแบบตรงต่อสำนักงานคณะกรรมการคุ้มครองผู้บริโภคโดยตรง 
 3. ธุรกิจตลาดแบบตรงที่มีหน้าที่ต้องจดทะเบียนต่อสำนักงานคณะกรรมการคุ้มครองผู้บริโภคตามพระราชบัญญัติขายตรง และตลาดแบบตรง พ.ศ. 2545 นั้น หมายรวมถึงบุคคลที่ทำการค้าขายสินค้าผ่านสื่ออื่นๆด้วย เช่น สื่อโทรศัพท์ โทรสาร หรือเครื่องมือสื่อสารอิเล็กทรอนิกส์ในรูปแบบอื่นๆ</t>
+  </si>
+  <si>
+    <t>การแชร์รูปภาพหรือข้อความต่างๆ เกี่ยวกับร้านค้าออนไลน์ของตนในพื้นที่โซเซียลมีเดียของผู้อื่นผิดกฎหมายนะครับ สามารถอ่านเพิ่มเติมได้ที่ https://www.sanook.com/campus/1401439/</t>
   </si>
 </sst>
 </file>
@@ -585,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -615,7 +615,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -634,7 +634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="105" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -642,7 +642,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="150" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -658,7 +658,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -666,7 +666,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="180" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -679,7 +679,7 @@
         <v>14</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add more res in บอทโง่ tag
</commit_message>
<xml_diff>
--- a/data/response.xlsx
+++ b/data/response.xlsx
@@ -5,17 +5,17 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Projects\baisd\chat_bot_team\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project_chatbot\chat_bot_team\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E0AF35-6B08-4CDB-9247-057C84ACEAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71A5BAF-56AC-4F00-AE14-7AFB349FCF55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t>tag</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>การแชร์รูปภาพหรือข้อความต่างๆ เกี่ยวกับร้านค้าออนไลน์ของตนในพื้นที่โซเซียลมีเดียของผู้อื่นผิดกฎหมายนะครับ สามารถอ่านเพิ่มเติมได้ที่ https://www.sanook.com/campus/1401439/</t>
+  </si>
+  <si>
+    <t>ซักหมัดป้ะ</t>
   </si>
 </sst>
 </file>
@@ -585,16 +588,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="77.6640625" customWidth="1"/>
+    <col min="2" max="2" width="77.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -602,7 +605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="135" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -610,7 +613,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -618,7 +621,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -626,7 +629,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -634,7 +637,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="105" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -642,7 +645,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="150" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -650,7 +653,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -658,7 +661,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -666,7 +669,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="180" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -674,7 +677,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="225" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -682,7 +685,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -690,7 +693,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -698,7 +701,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -706,7 +709,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -714,7 +717,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -722,7 +725,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -730,7 +733,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -738,7 +741,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -746,7 +749,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -754,7 +765,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -762,7 +773,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -770,7 +781,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -778,7 +789,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -786,7 +797,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -794,7 +805,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -802,7 +813,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -813,7 +824,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:B1 A4 A2 A3 A12:B31 A11 A10 A9 A8 A7 A6 A5" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:B1 A4 A2 A3 A12:B23 A11 A10 A9 A8 A7 A6 A5 A25:B27 A29:B31" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add more res to ทำอะไร tag
</commit_message>
<xml_diff>
--- a/data/response.xlsx
+++ b/data/response.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project_chatbot\chat_bot_team\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71A5BAF-56AC-4F00-AE14-7AFB349FCF55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECC76C6-B77A-4470-AE84-30A78CE1FFAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>tag</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>ซักหมัดป้ะ</t>
+  </si>
+  <si>
+    <t>ให้ความรู้เรื่องกฎหมายการขายของออนไลน์น้าบ</t>
   </si>
 </sst>
 </file>
@@ -773,6 +776,14 @@
         <v>29</v>
       </c>
     </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
create new res tag
</commit_message>
<xml_diff>
--- a/data/response.xlsx
+++ b/data/response.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project_chatbot\chat_bot_team\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129BBE72-FB4F-43CC-B54A-09DBD74644E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3EF8E00-47D4-4DBE-B08A-BD902BDA0E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
   <si>
     <t>tag</t>
   </si>
@@ -210,6 +210,12 @@
   </si>
   <si>
     <t>ให้ความรู้เรื่องกฎหมายการขายของออนไลน์น้าบ</t>
+  </si>
+  <si>
+    <t>เบื่อ</t>
+  </si>
+  <si>
+    <t>งั้นมาเล่นเกมส์ตอบคำถามกันถ้าตอบถูกหมด 3 ข้อจะได้รางวัลจากน้องบอทแหละ &lt;3 โอเค๊?</t>
   </si>
 </sst>
 </file>
@@ -589,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,6 +838,14 @@
         <v>43</v>
       </c>
     </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
create new tag res
</commit_message>
<xml_diff>
--- a/data/response.xlsx
+++ b/data/response.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project_chatbot\chat_bot_team\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3EF8E00-47D4-4DBE-B08A-BD902BDA0E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F01FF30-3FCD-4891-8D3F-034460303967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
   <si>
     <t>tag</t>
   </si>
@@ -215,7 +215,13 @@
     <t>เบื่อ</t>
   </si>
   <si>
-    <t>งั้นมาเล่นเกมส์ตอบคำถามกันถ้าตอบถูกหมด 3 ข้อจะได้รางวัลจากน้องบอทแหละ &lt;3 โอเค๊?</t>
+    <t>ตกลง</t>
+  </si>
+  <si>
+    <t>งั้นมาเล่นเกมส์ตอบคำถามกัน ตอบถูกทั้งหมด 3 ข้อและไม่ผิดเลยจะได้รางวัลจากน้องบอทแหละ &lt;3 โอเค๊?</t>
+  </si>
+  <si>
+    <t>ข้อ 1 ประเทศอะไรรวยที่สุดดด? เพราะอะไร?</t>
   </si>
 </sst>
 </file>
@@ -595,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,7 +849,15 @@
         <v>49</v>
       </c>
       <c r="B41" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>50</v>
+      </c>
+      <c r="B42" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add more tag res
</commit_message>
<xml_diff>
--- a/data/response.xlsx
+++ b/data/response.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project_chatbot\chat_bot_team\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748384FC-BAC2-4288-9742-C601BBD8ED4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED214F18-BB75-424A-ACAF-48E167E302CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="59">
   <si>
     <t>tag</t>
   </si>
@@ -234,6 +234,13 @@
   </si>
   <si>
     <t>ข้อ 3 ปีอะไรเอ่ย มีหลากสี?</t>
+  </si>
+  <si>
+    <t>ถูกสาม</t>
+  </si>
+  <si>
+    <t>ยินดีด้วยค้าบเตง ตอบถูกหมดเยย รับไปสำหรับรางวัลของคนเก่ง &lt;3
+https://www.youtube.com/watch?v=dQw4w9WgXcQ</t>
   </si>
 </sst>
 </file>
@@ -613,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,6 +895,14 @@
         <v>56</v>
       </c>
     </row>
+    <row r="45" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>57</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
add response for tag where
</commit_message>
<xml_diff>
--- a/data/response.xlsx
+++ b/data/response.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -766,9 +766,33 @@
         <v>อากาศดีมากก</v>
       </c>
     </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>where</v>
+      </c>
+      <c r="B59" t="str">
+        <v>i'm everywhere</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>where</v>
+      </c>
+      <c r="B60" t="str">
+        <v>i'm behind you ;)</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>where</v>
+      </c>
+      <c r="B61" t="str">
+        <v>In your Heart ♥♥♥</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B57"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B61"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>